<commit_message>
Assembler file updated, no issues yet
Have to compare with the given .hack files.
</commit_message>
<xml_diff>
--- a/nand2tetris/projects/06/add/Instructions.xlsx
+++ b/nand2tetris/projects/06/add/Instructions.xlsx
@@ -324,7 +324,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -333,15 +333,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -373,10 +369,10 @@
   <dimension ref="A2:I20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -561,13 +557,13 @@
       <c r="E10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>37</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -601,7 +597,7 @@
       <c r="C13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
@@ -674,7 +670,7 @@
       <c r="B20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>